<commit_message>
table with project properties, and brainstorming JSON schema to implement
</commit_message>
<xml_diff>
--- a/notes/ProjectMetadata/ProjectMetadataModel.xlsx
+++ b/notes/ProjectMetadata/ProjectMetadataModel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GithubC\iSamples\metadata\notes\ProjectMetadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D71821E8-01F8-46B9-A46D-CD8C2202B634}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE530EEB-09CC-44E3-A68F-EAFEE4E0BB0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8370" yWindow="2355" windowWidth="21405" windowHeight="14475" xr2:uid="{F1763673-EBBE-4CC1-855C-62B4E8209376}"/>
+    <workbookView xWindow="1635" yWindow="420" windowWidth="21405" windowHeight="15390" xr2:uid="{F1763673-EBBE-4CC1-855C-62B4E8209376}"/>
   </bookViews>
   <sheets>
     <sheet name="synthesis" sheetId="4" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">CitizenScience!$B$2:$B$76</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">synthesis!$C$1:$C$31</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">synthesis!$C$1:$C$30</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="412">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1002" uniqueCount="417">
   <si>
     <t>doiPrefix</t>
   </si>
@@ -1080,9 +1080,6 @@
     <t xml:space="preserve">i.e. scientists or academic departments using the data collected. One or more Agent objects </t>
   </si>
   <si>
-    <t>plannedOutcome</t>
-  </si>
-  <si>
     <t>purpose for the project. Should be related to plannedOutcome. ? Do there need to be two properties?</t>
   </si>
   <si>
@@ -1101,9 +1098,6 @@
     <t>Name of the project</t>
   </si>
   <si>
-    <t>part of</t>
-  </si>
-  <si>
     <t xml:space="preserve">link to a larger project that includes this project as a part. </t>
   </si>
   <si>
@@ -1173,9 +1167,6 @@
     <t>vocabulary (ISO639)</t>
   </si>
   <si>
-    <t>The planned outcome of the project, for comparison with actual outcome..?</t>
-  </si>
-  <si>
     <t>ISO8601 duration format</t>
   </si>
   <si>
@@ -2034,6 +2025,30 @@
   </si>
   <si>
     <t>related resource, contributor, alt identifier; Use dcat:qualified relation for related resource</t>
+  </si>
+  <si>
+    <t>responsibility[role=associatedParty]</t>
+  </si>
+  <si>
+    <t>responsibility[role=collaborator]</t>
+  </si>
+  <si>
+    <t>subject</t>
+  </si>
+  <si>
+    <t>The planned outcome of the project, for comparison with actual outcome..? Bundle in purpose text</t>
+  </si>
+  <si>
+    <t>related_resource[role = part of]</t>
+  </si>
+  <si>
+    <t>related_resource[role = has Part]</t>
+  </si>
+  <si>
+    <t>include in description</t>
+  </si>
+  <si>
+    <t>relatedResource [role=projectLandingPage]</t>
   </si>
 </sst>
 </file>
@@ -2146,7 +2161,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -2190,22 +2205,15 @@
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
@@ -2521,13 +2529,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE57A65D-E1FF-4330-ACAF-FCF2B938A48F}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:M40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="B9" sqref="B9:C29"/>
+      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2535,8 +2542,8 @@
     <col min="2" max="2" width="23.42578125" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
     <col min="4" max="4" width="59.85546875" customWidth="1"/>
-    <col min="8" max="8" width="19.42578125" style="20" customWidth="1"/>
-    <col min="9" max="9" width="42" customWidth="1"/>
+    <col min="8" max="8" width="19.42578125" customWidth="1"/>
+    <col min="9" max="9" width="72.140625" customWidth="1"/>
     <col min="10" max="10" width="18.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -2562,7 +2569,7 @@
       <c r="G1" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="H1" s="5" t="s">
         <v>338</v>
       </c>
       <c r="I1" s="5" t="s">
@@ -2572,123 +2579,117 @@
         <v>265</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="33" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>299</v>
+        <v>310</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>386</v>
-      </c>
-      <c r="D2" s="15" t="s">
-        <v>341</v>
+        <v>378</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>346</v>
       </c>
       <c r="E2" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G2" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>394</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>350</v>
+      </c>
+      <c r="E3" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="H2" s="15" t="s">
-        <v>85</v>
-      </c>
-      <c r="I2" s="6" t="s">
-        <v>86</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="K2" s="9"/>
-      <c r="L2" s="9"/>
-      <c r="M2" s="9"/>
-    </row>
-    <row r="3" spans="1:13" ht="49.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B3" s="6" t="s">
+      <c r="F3" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G3" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H3" s="6" t="s">
+        <v>181</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>182</v>
+      </c>
+      <c r="J3" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>382</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="6" t="s">
+        <v>135</v>
+      </c>
+      <c r="G4" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>187</v>
+      </c>
+      <c r="I4" s="6" t="s">
+        <v>188</v>
+      </c>
+      <c r="J4" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>296</v>
       </c>
-      <c r="C3" s="18" t="s">
-        <v>387</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="C5" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="D5" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="E3" s="6" t="s">
-        <v>372</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G3" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="H3" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="I3" s="6" t="s">
-        <v>72</v>
-      </c>
-      <c r="J3" s="10" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" ht="132" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B4" s="6" t="s">
-        <v>307</v>
-      </c>
-      <c r="C4" s="6" t="s">
-        <v>388</v>
-      </c>
-      <c r="D4" s="15" t="s">
-        <v>343</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>119</v>
-      </c>
-      <c r="I4" s="6" t="s">
-        <v>120</v>
-      </c>
-      <c r="J4" s="2" t="s">
-        <v>161</v>
-      </c>
-      <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
-      <c r="M4" s="9"/>
-    </row>
-    <row r="5" spans="1:13" ht="49.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="6" t="s">
-        <v>306</v>
-      </c>
-      <c r="C5" s="6" t="s">
-        <v>389</v>
-      </c>
-      <c r="D5" s="15" t="s">
-        <v>344</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="F5" s="6" t="s">
         <v>73</v>
@@ -2696,28 +2697,26 @@
       <c r="G5" s="6" t="s">
         <v>165</v>
       </c>
-      <c r="H5" s="15" t="s">
-        <v>116</v>
+      <c r="H5" s="6" t="s">
+        <v>71</v>
       </c>
       <c r="I5" s="6" t="s">
-        <v>117</v>
-      </c>
-      <c r="J5" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="J5" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="6" spans="1:13" ht="33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" ht="33" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="6" t="s">
-        <v>385</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C6" s="6"/>
       <c r="D6" s="6" t="s">
-        <v>188</v>
+        <v>345</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>3</v>
@@ -2728,221 +2727,224 @@
       <c r="G6" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H6" s="15" t="s">
-        <v>187</v>
+      <c r="H6" s="6" t="s">
+        <v>184</v>
       </c>
       <c r="I6" s="6" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="J6" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="132" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>327</v>
+        <v>411</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>384</v>
+        <v>389</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>205</v>
+        <v>347</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>377</v>
+        <v>372</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G7" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="H7" s="15" t="s">
-        <v>204</v>
+        <v>73</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>194</v>
       </c>
       <c r="I7" s="6" t="s">
-        <v>205</v>
+        <v>195</v>
       </c>
       <c r="J7" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="99" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="99" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B8" s="6" t="s">
-        <v>317</v>
+        <v>357</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>383</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>319</v>
+        <v>400</v>
+      </c>
+      <c r="D8" s="6" t="s">
+        <v>358</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>110</v>
+        <v>366</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H8" s="15" t="s">
-        <v>108</v>
-      </c>
-      <c r="I8" s="6" t="s">
-        <v>109</v>
-      </c>
-      <c r="J8" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" ht="66" x14ac:dyDescent="0.25">
+        <v>135</v>
+      </c>
+      <c r="G8" s="7" t="s">
+        <v>361</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>219</v>
+      </c>
+      <c r="I8" s="6"/>
+      <c r="J8" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" ht="33" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>305</v>
+        <v>334</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>382</v>
+        <v>402</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>373</v>
+        <v>355</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>73</v>
+        <v>135</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H9" s="15" t="s">
-        <v>102</v>
+        <v>361</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>224</v>
       </c>
       <c r="I9" s="6" t="s">
-        <v>103</v>
-      </c>
-      <c r="J9" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" ht="66" x14ac:dyDescent="0.25">
+        <v>225</v>
+      </c>
+      <c r="J9" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" ht="99" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B10" s="6" t="s">
-        <v>308</v>
+        <v>356</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>390</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>323</v>
+        <v>401</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>324</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>371</v>
+        <v>366</v>
       </c>
       <c r="F10" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H10" s="15" t="s">
-        <v>139</v>
+        <v>349</v>
+      </c>
+      <c r="H10" s="6" t="s">
+        <v>153</v>
       </c>
       <c r="I10" s="6" t="s">
-        <v>140</v>
+        <v>154</v>
       </c>
       <c r="J10" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="11" spans="1:13" ht="49.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" ht="132" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B11" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C11" s="6"/>
+        <v>409</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>385</v>
+      </c>
       <c r="D11" s="6" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>3</v>
+        <v>366</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G11" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="H11" s="15" t="s">
-        <v>184</v>
+        <v>73</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>119</v>
       </c>
       <c r="I11" s="6" t="s">
-        <v>185</v>
-      </c>
-      <c r="J11" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" ht="99" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+      <c r="J11" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+    </row>
+    <row r="12" spans="1:13" ht="33" x14ac:dyDescent="0.25">
       <c r="A12" s="6" t="s">
-        <v>167</v>
+        <v>70</v>
       </c>
       <c r="B12" s="6" t="s">
-        <v>309</v>
+        <v>410</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>391</v>
+        <v>386</v>
       </c>
       <c r="D12" s="6" t="s">
-        <v>326</v>
+        <v>344</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="F12" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H12" s="15" t="s">
-        <v>168</v>
+        <v>165</v>
+      </c>
+      <c r="H12" s="6" t="s">
+        <v>116</v>
       </c>
       <c r="I12" s="6" t="s">
-        <v>169</v>
-      </c>
-      <c r="J12" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" ht="33" hidden="1" x14ac:dyDescent="0.25">
+        <v>117</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="33" x14ac:dyDescent="0.25">
       <c r="A13" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B13" s="6" t="s">
-        <v>310</v>
+        <v>315</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>381</v>
+        <v>376</v>
       </c>
       <c r="D13" s="6" t="s">
-        <v>347</v>
+        <v>316</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="F13" s="6" t="s">
         <v>135</v>
@@ -2950,282 +2952,287 @@
       <c r="G13" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H13" s="15" t="s">
-        <v>170</v>
+      <c r="H13" s="6" t="s">
+        <v>197</v>
       </c>
       <c r="I13" s="6" t="s">
-        <v>171</v>
+        <v>198</v>
       </c>
       <c r="J13" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="14" spans="1:13" ht="82.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
       <c r="A14" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>194</v>
+        <v>318</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>392</v>
+        <v>375</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>348</v>
+        <v>320</v>
       </c>
       <c r="E14" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G14" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H14" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="I14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>317</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>380</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="E15" s="6" t="s">
+        <v>110</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G15" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H15" s="6" t="s">
+        <v>108</v>
+      </c>
+      <c r="I15" s="6" t="s">
+        <v>109</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>381</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>205</v>
+      </c>
+      <c r="E16" s="6" t="s">
         <v>374</v>
-      </c>
-      <c r="F14" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G14" s="6" t="s">
-        <v>361</v>
-      </c>
-      <c r="H14" s="15" t="s">
-        <v>194</v>
-      </c>
-      <c r="I14" s="6" t="s">
-        <v>195</v>
-      </c>
-      <c r="J14" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" ht="49.5" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B15" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>393</v>
-      </c>
-      <c r="D15" s="6" t="s">
-        <v>362</v>
-      </c>
-      <c r="E15" s="6" t="s">
-        <v>375</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G15" s="7" t="s">
-        <v>164</v>
-      </c>
-      <c r="H15" s="15" t="s">
-        <v>213</v>
-      </c>
-      <c r="I15" s="6" t="s">
-        <v>214</v>
-      </c>
-      <c r="J15" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="16" spans="1:13" ht="132" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B16" s="6" t="s">
-        <v>303</v>
-      </c>
-      <c r="C16" s="6" t="s">
-        <v>394</v>
-      </c>
-      <c r="D16" s="6" t="s">
-        <v>364</v>
-      </c>
-      <c r="E16" s="6" t="s">
-        <v>121</v>
       </c>
       <c r="F16" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="G16" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="H16" s="15" t="s">
-        <v>246</v>
+      <c r="G16" s="7" t="s">
+        <v>166</v>
+      </c>
+      <c r="H16" s="6" t="s">
+        <v>204</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>247</v>
+        <v>205</v>
       </c>
       <c r="J16" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="82.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" ht="66" x14ac:dyDescent="0.25">
       <c r="A17" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B17" s="6" t="s">
-        <v>303</v>
+        <v>305</v>
       </c>
       <c r="C17" s="6" t="s">
-        <v>395</v>
+        <v>379</v>
       </c>
       <c r="D17" s="6" t="s">
+        <v>371</v>
+      </c>
+      <c r="E17" s="6" t="s">
+        <v>370</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G17" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="E17" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F17" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G17" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="H17" s="15" t="s">
-        <v>216</v>
+      <c r="H17" s="6" t="s">
+        <v>102</v>
       </c>
       <c r="I17" s="6" t="s">
-        <v>217</v>
-      </c>
-      <c r="J17" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" ht="66" hidden="1" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="66" x14ac:dyDescent="0.25">
       <c r="A18" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B18" s="6" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>396</v>
+        <v>387</v>
       </c>
       <c r="D18" s="6" t="s">
-        <v>314</v>
+        <v>323</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>176</v>
+        <v>369</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G18" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="H18" s="15" t="s">
-        <v>178</v>
+        <v>73</v>
+      </c>
+      <c r="G18" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="H18" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="I18" s="6" t="s">
-        <v>179</v>
-      </c>
-      <c r="J18" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" ht="49.5" x14ac:dyDescent="0.25">
+        <v>140</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="33" x14ac:dyDescent="0.25">
       <c r="A19" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B19" s="6" t="s">
-        <v>4</v>
+        <v>299</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>397</v>
+        <v>383</v>
       </c>
       <c r="D19" s="6" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>3</v>
       </c>
       <c r="F19" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G19" s="6" t="s">
+        <v>165</v>
+      </c>
+      <c r="H19" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="I19" s="6" t="s">
+        <v>86</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+    </row>
+    <row r="20" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="C20" s="6" t="s">
+        <v>390</v>
+      </c>
+      <c r="D20" s="6" t="s">
+        <v>360</v>
+      </c>
+      <c r="E20" s="6" t="s">
+        <v>373</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>164</v>
+      </c>
+      <c r="H20" s="6" t="s">
+        <v>213</v>
+      </c>
+      <c r="I20" s="6" t="s">
+        <v>214</v>
+      </c>
+      <c r="J20" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="132" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" s="6" t="s">
+        <v>303</v>
+      </c>
+      <c r="C21" s="6" t="s">
+        <v>391</v>
+      </c>
+      <c r="D21" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="E21" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="F21" s="6" t="s">
         <v>135</v>
       </c>
-      <c r="G19" s="7" t="s">
-        <v>166</v>
-      </c>
-      <c r="H19" s="15" t="s">
-        <v>181</v>
-      </c>
-      <c r="I19" s="6" t="s">
-        <v>182</v>
-      </c>
-      <c r="J19" s="10" t="s">
+      <c r="G21" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="H21" s="6" t="s">
+        <v>246</v>
+      </c>
+      <c r="I21" s="6" t="s">
+        <v>247</v>
+      </c>
+      <c r="J21" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="66" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B20" s="6" t="s">
-        <v>352</v>
-      </c>
-      <c r="C20" s="6" t="s">
-        <v>398</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>353</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>370</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G20" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H20" s="15" t="s">
-        <v>75</v>
-      </c>
-      <c r="I20" s="6" t="s">
-        <v>76</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" ht="33" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="6" t="s">
-        <v>345</v>
-      </c>
-      <c r="C21" s="18"/>
-      <c r="D21" s="15" t="s">
-        <v>376</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G21" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H21" s="15" t="s">
-        <v>83</v>
-      </c>
-      <c r="I21" s="6" t="s">
-        <v>84</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" ht="198" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A22" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B22" s="6" t="s">
-        <v>300</v>
+        <v>303</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>380</v>
+        <v>392</v>
       </c>
       <c r="D22" s="6" t="s">
-        <v>354</v>
+        <v>348</v>
       </c>
       <c r="E22" s="6" t="s">
         <v>3</v>
@@ -3233,280 +3240,278 @@
       <c r="F22" s="6" t="s">
         <v>73</v>
       </c>
-      <c r="G22" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H22" s="15" t="s">
-        <v>260</v>
+      <c r="G22" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="H22" s="6" t="s">
+        <v>216</v>
       </c>
       <c r="I22" s="6" t="s">
-        <v>261</v>
+        <v>217</v>
       </c>
       <c r="J22" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="23" spans="1:10" ht="49.5" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:13" ht="66" x14ac:dyDescent="0.25">
       <c r="A23" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B23" s="6" t="s">
+        <v>413</v>
+      </c>
+      <c r="C23" s="6" t="s">
+        <v>395</v>
+      </c>
+      <c r="D23" s="16" t="s">
+        <v>351</v>
+      </c>
+      <c r="E23" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F23" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G23" s="6" t="s">
+        <v>164</v>
+      </c>
+      <c r="H23" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="I23" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="33" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B24" s="6"/>
+      <c r="C24" s="17"/>
+      <c r="D24" s="6" t="s">
+        <v>412</v>
+      </c>
+      <c r="E24" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F24" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G24" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="H24" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="I24" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="115.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="6" t="s">
+        <v>415</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>377</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>352</v>
+      </c>
+      <c r="E25" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F25" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G25" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="H25" s="6" t="s">
+        <v>260</v>
+      </c>
+      <c r="I25" s="6" t="s">
+        <v>261</v>
+      </c>
+      <c r="J25" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>167</v>
+      </c>
+      <c r="B26" s="6" t="s">
+        <v>414</v>
+      </c>
+      <c r="C26" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="D26" s="6" t="s">
+        <v>326</v>
+      </c>
+      <c r="E26" s="6" t="s">
+        <v>368</v>
+      </c>
+      <c r="F26" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G26" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="H26" s="6" t="s">
+        <v>168</v>
+      </c>
+      <c r="I26" s="6" t="s">
+        <v>169</v>
+      </c>
+      <c r="J26" s="10" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="49.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="B27" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="C23" s="6" t="s">
-        <v>399</v>
-      </c>
-      <c r="D23" s="6" t="s">
+      <c r="C27" s="6" t="s">
+        <v>396</v>
+      </c>
+      <c r="D27" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="E23" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="F23" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G23" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H23" s="15" t="s">
+      <c r="E27" s="6" t="s">
+        <v>365</v>
+      </c>
+      <c r="F27" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="G27" s="6" t="s">
+        <v>349</v>
+      </c>
+      <c r="H27" s="6" t="s">
         <v>235</v>
       </c>
-      <c r="I23" s="6" t="s">
+      <c r="I27" s="6" t="s">
         <v>236</v>
       </c>
-      <c r="J23" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" ht="70.5" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B24" s="6" t="s">
-        <v>329</v>
-      </c>
-      <c r="C24" s="6" t="s">
-        <v>400</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G24" s="7" t="s">
-        <v>350</v>
-      </c>
-      <c r="H24" s="15" t="s">
-        <v>209</v>
-      </c>
-      <c r="I24" s="6" t="s">
-        <v>210</v>
-      </c>
-      <c r="J24" s="10" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B25" s="6" t="s">
-        <v>355</v>
-      </c>
-      <c r="C25" s="6" t="s">
-        <v>401</v>
-      </c>
-      <c r="D25" s="6" t="s">
-        <v>356</v>
-      </c>
-      <c r="E25" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G25" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H25" s="15" t="s">
-        <v>92</v>
-      </c>
-      <c r="I25" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="J25" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" ht="82.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="6"/>
-      <c r="B26" s="6" t="s">
-        <v>365</v>
-      </c>
-      <c r="C26" s="6" t="s">
-        <v>402</v>
-      </c>
-      <c r="D26" s="6" t="s">
-        <v>366</v>
-      </c>
-      <c r="E26" s="6" t="s">
-        <v>367</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>73</v>
-      </c>
-      <c r="G26" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H26" s="15"/>
-      <c r="I26" s="6"/>
-      <c r="J26" s="2"/>
-    </row>
-    <row r="27" spans="1:10" ht="99" x14ac:dyDescent="0.25">
-      <c r="A27" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="B27" s="6" t="s">
-        <v>359</v>
-      </c>
-      <c r="C27" s="6" t="s">
-        <v>403</v>
-      </c>
-      <c r="D27" s="6" t="s">
-        <v>360</v>
-      </c>
-      <c r="E27" s="6" t="s">
-        <v>368</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G27" s="7" t="s">
-        <v>363</v>
-      </c>
-      <c r="H27" s="15" t="s">
-        <v>219</v>
-      </c>
-      <c r="I27" s="6"/>
       <c r="J27" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="33" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:13" ht="70.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>334</v>
+        <v>416</v>
       </c>
       <c r="C28" s="6" t="s">
-        <v>405</v>
+        <v>397</v>
       </c>
       <c r="D28" s="6" t="s">
-        <v>357</v>
+        <v>210</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F28" s="6" t="s">
-        <v>135</v>
-      </c>
-      <c r="G28" s="6" t="s">
-        <v>363</v>
-      </c>
-      <c r="H28" s="15" t="s">
-        <v>224</v>
+        <v>73</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>349</v>
+      </c>
+      <c r="H28" s="6" t="s">
+        <v>209</v>
       </c>
       <c r="I28" s="6" t="s">
-        <v>225</v>
+        <v>210</v>
       </c>
       <c r="J28" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="99" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" ht="82.5" x14ac:dyDescent="0.25">
       <c r="A29" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>358</v>
+        <v>353</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>404</v>
+        <v>398</v>
       </c>
       <c r="D29" s="6" t="s">
-        <v>324</v>
+        <v>354</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>368</v>
+        <v>365</v>
       </c>
       <c r="F29" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G29" s="6" t="s">
-        <v>350</v>
-      </c>
-      <c r="H29" s="15" t="s">
-        <v>153</v>
+        <v>349</v>
+      </c>
+      <c r="H29" s="6" t="s">
+        <v>92</v>
       </c>
       <c r="I29" s="6" t="s">
-        <v>154</v>
+        <v>93</v>
       </c>
       <c r="J29" s="2" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="66" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="6" t="s">
-        <v>70</v>
-      </c>
+    <row r="30" spans="1:13" ht="82.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6"/>
       <c r="B30" s="6" t="s">
-        <v>318</v>
+        <v>363</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>378</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>320</v>
+        <v>399</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>364</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>110</v>
+        <v>365</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>73</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>164</v>
-      </c>
-      <c r="H30" s="15" t="s">
-        <v>111</v>
-      </c>
-      <c r="I30" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" ht="33" hidden="1" x14ac:dyDescent="0.25">
+        <v>349</v>
+      </c>
+      <c r="H30" s="6"/>
+      <c r="I30" s="6"/>
+      <c r="J30" s="2"/>
+    </row>
+    <row r="31" spans="1:13" ht="66" x14ac:dyDescent="0.25">
       <c r="A31" s="6" t="s">
         <v>70</v>
       </c>
       <c r="B31" s="6" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>379</v>
+        <v>393</v>
       </c>
       <c r="D31" s="6" t="s">
-        <v>316</v>
+        <v>314</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>369</v>
+        <v>176</v>
       </c>
       <c r="F31" s="6" t="s">
         <v>135</v>
@@ -3514,11 +3519,11 @@
       <c r="G31" s="7" t="s">
         <v>166</v>
       </c>
-      <c r="H31" s="15" t="s">
-        <v>197</v>
+      <c r="H31" s="6" t="s">
+        <v>178</v>
       </c>
       <c r="I31" s="6" t="s">
-        <v>198</v>
+        <v>179</v>
       </c>
       <c r="J31" s="10" t="s">
         <v>264</v>
@@ -3526,13 +3531,13 @@
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C34">
-        <f>COUNTA(C2:C31)</f>
-        <v>28</v>
+        <f>COUNTA(C11:C30)</f>
+        <v>19</v>
       </c>
     </row>
     <row r="35" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
-        <v>406</v>
+        <v>403</v>
       </c>
       <c r="C35">
         <v>22</v>
@@ -3540,7 +3545,7 @@
     </row>
     <row r="36" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
-        <v>407</v>
+        <v>404</v>
       </c>
       <c r="C36">
         <v>18</v>
@@ -3548,7 +3553,7 @@
     </row>
     <row r="37" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
-        <v>408</v>
+        <v>405</v>
       </c>
       <c r="C37">
         <v>2</v>
@@ -3556,41 +3561,28 @@
     </row>
     <row r="39" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
-        <v>409</v>
+        <v>406</v>
       </c>
       <c r="C39">
         <v>6</v>
       </c>
       <c r="D39" t="s">
-        <v>411</v>
+        <v>408</v>
       </c>
     </row>
     <row r="40" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
-        <v>410</v>
+        <v>407</v>
       </c>
       <c r="C40">
         <v>9</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C31" xr:uid="{DE57A65D-E1FF-4330-ACAF-FCF2B938A48F}">
-    <filterColumn colId="0">
-      <filters>
-        <filter val="dcterms:title; RAID:activity name; datacite:titles/title; schema:name"/>
-        <filter val="RAID:Instrument; schema:instrument"/>
-        <filter val="RAID:Journal articles, pre-prints, conference papers; datacite:relatedIdentifier[ some type…]; dcat:qualifiedRelation"/>
-        <filter val="RAID:Projects; datacite:relatedIdentifer[type=hasPart]; schema:hasPart; dcterms:hasPart"/>
-        <filter val="RAID:Research contributor; datacite:contributor[type=&quot;ProjectLeader&quot;,&quot;ProjectManager&quot;, &quot;ProjectMember&quot;, &quot;Researcher&quot;,&quot;ResearchGroup&quot;]; schema:member;"/>
-        <filter val="RAID:Research grant; RAID:Funding organization; schema:funding/Grant; datacite:fundingReferences"/>
-        <filter val="RAID:Research organization; datacite:contributor[type = Sponsor, HostingInstitution]; schema:sponsor"/>
-        <filter val="RAID:Stored data, RAID: Physical specimen; datacite:relatedIdentifier[ some type…]; dcat:qualifiedRelation"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:J31">
-    <sortCondition ref="B2:B31"/>
-    <sortCondition ref="H2:H31"/>
+  <autoFilter ref="C1:C30" xr:uid="{DE57A65D-E1FF-4330-ACAF-FCF2B938A48F}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A11:J30">
+    <sortCondition ref="B11:B30"/>
+    <sortCondition ref="H11:H30"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -3781,8 +3773,8 @@
       <c r="C3" s="14" t="s">
         <v>71</v>
       </c>
-      <c r="D3" s="15"/>
-      <c r="E3" s="15" t="s">
+      <c r="D3" s="6"/>
+      <c r="E3" s="6" t="s">
         <v>293</v>
       </c>
       <c r="F3" s="6" t="s">
@@ -3817,8 +3809,8 @@
       <c r="C4" s="14" t="s">
         <v>75</v>
       </c>
-      <c r="D4" s="15"/>
-      <c r="E4" s="15" t="s">
+      <c r="D4" s="6"/>
+      <c r="E4" s="6" t="s">
         <v>294</v>
       </c>
       <c r="F4" s="6" t="s">
@@ -3931,8 +3923,8 @@
       <c r="C8" s="14" t="s">
         <v>83</v>
       </c>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
       <c r="F8" s="6" t="s">
         <v>84</v>
       </c>
@@ -3965,8 +3957,8 @@
       <c r="C9" s="14" t="s">
         <v>85</v>
       </c>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
       <c r="F9" s="6" t="s">
         <v>86</v>
       </c>
@@ -3996,8 +3988,8 @@
       <c r="C10" s="14" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="15"/>
-      <c r="E10" s="15"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
       <c r="F10" s="6" t="s">
         <v>89</v>
       </c>
@@ -4203,8 +4195,8 @@
       <c r="C17" s="14" t="s">
         <v>108</v>
       </c>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15" t="s">
+      <c r="D17" s="6"/>
+      <c r="E17" s="6" t="s">
         <v>319</v>
       </c>
       <c r="F17" s="6" t="s">
@@ -4234,8 +4226,8 @@
       <c r="C18" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15" t="s">
+      <c r="D18" s="6"/>
+      <c r="E18" s="6" t="s">
         <v>320</v>
       </c>
       <c r="F18" s="6" t="s">
@@ -4265,8 +4257,8 @@
       <c r="C19" s="14" t="s">
         <v>113</v>
       </c>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15" t="s">
+      <c r="D19" s="6"/>
+      <c r="E19" s="6" t="s">
         <v>321</v>
       </c>
       <c r="F19" s="6" t="s">
@@ -4298,8 +4290,8 @@
       <c r="C20" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
       <c r="F20" s="6" t="s">
         <v>117</v>
       </c>
@@ -4329,8 +4321,8 @@
       <c r="C21" s="14" t="s">
         <v>119</v>
       </c>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15" t="s">
+      <c r="D21" s="6"/>
+      <c r="E21" s="6" t="s">
         <v>322</v>
       </c>
       <c r="F21" s="6" t="s">
@@ -4537,8 +4529,8 @@
       <c r="C29" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15" t="s">
+      <c r="D29" s="6"/>
+      <c r="E29" s="6" t="s">
         <v>323</v>
       </c>
       <c r="F29" s="6" t="s">
@@ -4871,7 +4863,7 @@
         <v>70</v>
       </c>
       <c r="B42" s="6"/>
-      <c r="C42" s="15" t="s">
+      <c r="C42" s="6" t="s">
         <v>174</v>
       </c>
       <c r="D42" s="6"/>
@@ -4902,7 +4894,7 @@
       <c r="B43" s="6" t="s">
         <v>311</v>
       </c>
-      <c r="C43" s="16" t="s">
+      <c r="C43" s="15" t="s">
         <v>178</v>
       </c>
       <c r="D43" s="6"/>
@@ -5419,7 +5411,7 @@
         <v>70</v>
       </c>
       <c r="B60" s="6"/>
-      <c r="C60" s="15" t="s">
+      <c r="C60" s="6" t="s">
         <v>222</v>
       </c>
       <c r="D60" s="6"/>

</xml_diff>